<commit_message>
Actualizaci[on Certificaci[on, arreglo de descarga de detalle
</commit_message>
<xml_diff>
--- a/Automatizacion_Banrural/Data/Input/Empresas.xlsx
+++ b/Automatizacion_Banrural/Data/Input/Empresas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Propa34653\Desktop\EY\Banrural\Automatizacion_Banrural\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C613A5-04EF-4553-A305-724FC9709B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5074CC7D-2011-4D91-B3C4-86FFACD769F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="3555" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="3900" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>COBRO COSMETICA GLOBAL</t>
   </si>
   <si>
-    <t>PAGO TELGUA EN LINEA</t>
-  </si>
-  <si>
     <t>TELGUA COMPRA DE TIEMPO DE AIRE</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>B5</t>
+  </si>
+  <si>
+    <t>CxCAjena - PAGO TELGUA EN LINEA</t>
   </si>
 </sst>
 </file>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,7 +396,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -432,33 +432,30 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:A4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>